<commit_message>
Update results file with pvalues from new model runs
</commit_message>
<xml_diff>
--- a/nectar analysis/analysis/model_results_summary.xlsx
+++ b/nectar analysis/analysis/model_results_summary.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Audrey McCombs\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7908"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Balsamroot</t>
   </si>
@@ -47,25 +42,37 @@
     <t>Buckwheat</t>
   </si>
   <si>
-    <t>lmer(BRIX ~ treatment * year + (1|plot/plant), data = balssugboth)</t>
-  </si>
-  <si>
-    <t>lmer(volume ~ treatment * year + (1|plot/plant), data = balsvolboth)</t>
-  </si>
-  <si>
-    <t>lmer(mass ~ treatment * year + (1|plot/plant), data = balssugboth)</t>
-  </si>
-  <si>
-    <t>lmer(volume ~ treatment * year + (1|plot), data = buckvolboth)</t>
-  </si>
-  <si>
-    <t>lmer(BRIX ~ treatment * year + (1|plot), data = bucksugboth)</t>
-  </si>
-  <si>
-    <t>lmer(mass ~ treatment * year + (1|plot), data = bucksugboth)</t>
-  </si>
-  <si>
     <t>These are LS means p-values from the indicated models</t>
+  </si>
+  <si>
+    <t>lmer(BRIX ~ treatment * year +(1|plot/plant) + (1|year:date), data = balssugboth)</t>
+  </si>
+  <si>
+    <t>lmer(lnmass ~ treatment * year + (1|plot/plant) + (1|year:date), data = balssugboth)</t>
+  </si>
+  <si>
+    <t>lmer(lnvol ~ treatment * year + (1|plot/plant) + (1|year:date), data = balsvolboth)</t>
+  </si>
+  <si>
+    <t>lmer(BRIX ~ treatment * year + (1|plot) + (1|year:date), data = bucksugboth)</t>
+  </si>
+  <si>
+    <t>lmer(lnmass ~ treatment * year + (1|plot) + (1|year:date), data = bucksugboth)</t>
+  </si>
+  <si>
+    <t>lmer(lnvol ~ treatment * year + (1|plot) +(1|year:date), data = buckvolboth)</t>
+  </si>
+  <si>
+    <t>Presence/absence</t>
+  </si>
+  <si>
+    <t>glmer(necpres ~ treatment * year + (1|plot/plant) + (1| year:date), data = balsam, family = binomial)</t>
+  </si>
+  <si>
+    <t>glmer(necpres ~ treatment + (1|plot) + (1|date), data = buckwt, family = binomial)</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -73,7 +80,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -92,7 +99,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +109,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -118,12 +131,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -184,7 +199,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -219,7 +234,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -396,7 +411,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -404,13 +419,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
@@ -437,16 +452,16 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>0.14979999999999999</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="C2" s="1">
-        <v>0.89500000000000002</v>
+        <v>0.80700000000000005</v>
       </c>
       <c r="D2" s="1">
-        <v>0.26319999999999999</v>
+        <v>0.60160000000000002</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -454,16 +469,16 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>1.9199999999999998E-2</v>
+        <v>3.6499999999999998E-2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.21429999999999999</v>
+        <v>0.39450000000000002</v>
       </c>
       <c r="D3" s="3">
-        <v>4.2000000000000003E-2</v>
+        <v>9.3200000000000005E-2</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -471,13 +486,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>0.41970000000000002</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.71799999999999997</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.46029999999999999</v>
+        <v>0.3896</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.1013</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.1024</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -492,17 +507,17 @@
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7">
-        <v>0.14979999999999999</v>
+      <c r="B7" s="4">
+        <v>1.0699999999999999E-2</v>
       </c>
       <c r="C7" s="1">
-        <v>0.89500000000000002</v>
-      </c>
-      <c r="D7">
-        <v>0.26319999999999999</v>
+        <v>0.55930000000000002</v>
+      </c>
+      <c r="D7" s="6">
+        <v>7.7100000000000002E-2</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -513,10 +528,10 @@
         <v>1.1999999999999999E-3</v>
       </c>
       <c r="C8" s="1">
-        <v>0.32400000000000001</v>
+        <v>0.26869999999999999</v>
       </c>
       <c r="D8" s="4">
-        <v>1.9699999999999999E-2</v>
+        <v>1.8100000000000002E-2</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
@@ -527,21 +542,60 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>0.11409999999999999</v>
+        <v>0.22370000000000001</v>
       </c>
       <c r="C9" s="1">
-        <v>0.74180000000000001</v>
+        <v>0.40489999999999998</v>
       </c>
       <c r="D9">
-        <v>0.28120000000000001</v>
+        <v>0.25209999999999999</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>13</v>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="6">
+        <v>7.6100000000000001E-2</v>
+      </c>
+      <c r="C12">
+        <v>0.73770000000000002</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.1115</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>0.4093</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Box plots for Buck and Bals models
</commit_message>
<xml_diff>
--- a/nectar analysis/analysis/model_results_summary.xlsx
+++ b/nectar analysis/analysis/model_results_summary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="77">
   <si>
     <t>Balsamroot</t>
   </si>
@@ -73,6 +73,183 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Number of Flowers</t>
+  </si>
+  <si>
+    <t>glmer(year15 ~ treatment + (1|plantid) + (1|plot), data = flowers, family = poisson)</t>
+  </si>
+  <si>
+    <t>&lt;.0001</t>
+  </si>
+  <si>
+    <t>glmer(year16 ~ treatment + (1|plantid) + (1|plot), data = flowers, family = poisson)</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>Estimates (*on log scale)</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Balsamroot BRIX 2015</t>
+  </si>
+  <si>
+    <t>C: 19.70</t>
+  </si>
+  <si>
+    <t>H: 25.67</t>
+  </si>
+  <si>
+    <t>C: 3.14</t>
+  </si>
+  <si>
+    <t>H: 2.93</t>
+  </si>
+  <si>
+    <t>Balsamroot BRIX 2015 and 2016</t>
+  </si>
+  <si>
+    <t>C: 23.75</t>
+  </si>
+  <si>
+    <t>H: 27.73</t>
+  </si>
+  <si>
+    <t>C: 2.42</t>
+  </si>
+  <si>
+    <t>H: 2.39</t>
+  </si>
+  <si>
+    <t>Balsamroot sugar mass 2016</t>
+  </si>
+  <si>
+    <t>C*:-3.38</t>
+  </si>
+  <si>
+    <t>H*:-3.13</t>
+  </si>
+  <si>
+    <t>C*:0.18</t>
+  </si>
+  <si>
+    <t>H*:0.18</t>
+  </si>
+  <si>
+    <t>Balsamroot sugar mass 2015 and 2016</t>
+  </si>
+  <si>
+    <t>C*:-3.06</t>
+  </si>
+  <si>
+    <t>H*:-2.85</t>
+  </si>
+  <si>
+    <t>C*:0.14</t>
+  </si>
+  <si>
+    <t>H*:0.12</t>
+  </si>
+  <si>
+    <t>Buckwheat volume 2015</t>
+  </si>
+  <si>
+    <t>C*:-0.97</t>
+  </si>
+  <si>
+    <t>H*:-1.26</t>
+  </si>
+  <si>
+    <t>C*:0.12</t>
+  </si>
+  <si>
+    <t>Buckwheat volume 2015 and 2016</t>
+  </si>
+  <si>
+    <t>C*:-1.85</t>
+  </si>
+  <si>
+    <t>H*:-2.02</t>
+  </si>
+  <si>
+    <t>C*:0.11</t>
+  </si>
+  <si>
+    <t>H*:0.11</t>
+  </si>
+  <si>
+    <t>Buckwheat BRIX 2015</t>
+  </si>
+  <si>
+    <t>C: 45.42</t>
+  </si>
+  <si>
+    <t>H: 54.16</t>
+  </si>
+  <si>
+    <t>C: 2.96</t>
+  </si>
+  <si>
+    <t>H: 2.96</t>
+  </si>
+  <si>
+    <t>Buckwheat BRIX 2015 and 2016</t>
+  </si>
+  <si>
+    <t>C: 50.66</t>
+  </si>
+  <si>
+    <t>H: 56.24</t>
+  </si>
+  <si>
+    <t>C: 2.60</t>
+  </si>
+  <si>
+    <t>H: 2.60</t>
+  </si>
+  <si>
+    <t>Balsamroot presence/absence 2015</t>
+  </si>
+  <si>
+    <t>C: 55% present</t>
+  </si>
+  <si>
+    <t>H: 61% present</t>
+  </si>
+  <si>
+    <t>Balsamroot number of flowers 2015</t>
+  </si>
+  <si>
+    <t>C: -0.22</t>
+  </si>
+  <si>
+    <t>H: 0.96</t>
+  </si>
+  <si>
+    <t>C: -0.66</t>
+  </si>
+  <si>
+    <t>H: 2.27</t>
+  </si>
+  <si>
+    <t>Balsamroot number of flowers 2016</t>
+  </si>
+  <si>
+    <t>&lt;0.0001</t>
+  </si>
+  <si>
+    <t>C: 1.12</t>
+  </si>
+  <si>
+    <t>C: 0.18</t>
+  </si>
+  <si>
+    <t>H: 0.24</t>
   </si>
 </sst>
 </file>
@@ -80,7 +257,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -133,12 +310,14 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,28 +598,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="4" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="2">
         <v>2015</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="2">
         <v>2016</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
@@ -451,13 +631,13 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>0.30499999999999999</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>0.80700000000000005</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>0.60160000000000002</v>
       </c>
       <c r="E2" t="s">
@@ -471,7 +651,7 @@
       <c r="B3" s="3">
         <v>3.6499999999999998E-2</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>0.39450000000000002</v>
       </c>
       <c r="D3" s="3">
@@ -485,13 +665,13 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>0.3896</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>0.1013</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>0.1024</v>
       </c>
       <c r="E4" t="s">
@@ -499,7 +679,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -507,13 +687,13 @@
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>1.0699999999999999E-2</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>0.55930000000000002</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="4">
         <v>7.7100000000000002E-2</v>
       </c>
       <c r="E7" t="s">
@@ -524,13 +704,13 @@
       <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>0.26869999999999999</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>1.8100000000000002E-2</v>
       </c>
       <c r="E8" t="s">
@@ -541,13 +721,13 @@
       <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>0.22370000000000001</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>0.40489999999999998</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>0.25209999999999999</v>
       </c>
       <c r="E9" t="s">
@@ -555,7 +735,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -563,13 +743,13 @@
       <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="4">
         <v>7.6100000000000001E-2</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>0.73770000000000002</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>0.1115</v>
       </c>
       <c r="E12" t="s">
@@ -580,22 +760,306 @@
       <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>0.4093</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E13" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D16" t="s">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.35E-2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D19" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="2">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="6"/>
+      <c r="C23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="2">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="6"/>
+      <c r="C25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="6"/>
+      <c r="C27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="6"/>
+      <c r="C29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="6"/>
+      <c r="C31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="2">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="6"/>
+      <c r="C33" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
+      <c r="C35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="6"/>
+      <c r="C37" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="6"/>
+      <c r="C39" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="2">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="6"/>
+      <c r="C41" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C43" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>